<commit_message>
files update no change
</commit_message>
<xml_diff>
--- a/Data/W4TRaC-BQE-overview.xlsx
+++ b/Data/W4TRaC-BQE-overview.xlsx
@@ -1,106 +1,126 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <workbookPr date1904="false"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uapt33090-my.sharepoint.com/personal/heliana_teixeira_ua_pt/Documents/Rdir/WFD-TRaC-data-upto2022/Data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="6" documentId="11_ADBEB2384E316FF43034A55A17DB0B61925963B6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{835831DC-21DC-D84D-9A18-C877B93AF6D3}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="15840" yWindow="1560" windowWidth="10000" windowHeight="14140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
-    <t xml:space="preserve"/>
-  </si>
-  <si>
-    <t xml:space="preserve">CW</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TW</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UK</t>
+    <t/>
+  </si>
+  <si>
+    <t>CW</t>
+  </si>
+  <si>
+    <t>TW</t>
+  </si>
+  <si>
+    <t>BE</t>
+  </si>
+  <si>
+    <t>BG</t>
+  </si>
+  <si>
+    <t>CY</t>
+  </si>
+  <si>
+    <t>DE</t>
+  </si>
+  <si>
+    <t>DK</t>
+  </si>
+  <si>
+    <t>EE</t>
+  </si>
+  <si>
+    <t>EL</t>
+  </si>
+  <si>
+    <t>ES</t>
+  </si>
+  <si>
+    <t>FI</t>
+  </si>
+  <si>
+    <t>FR</t>
+  </si>
+  <si>
+    <t>HR</t>
+  </si>
+  <si>
+    <t>IE</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>LT</t>
+  </si>
+  <si>
+    <t>LV</t>
+  </si>
+  <si>
+    <t>MT</t>
+  </si>
+  <si>
+    <t>NL</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>PL</t>
+  </si>
+  <si>
+    <t>PT</t>
+  </si>
+  <si>
+    <t>RO</t>
+  </si>
+  <si>
+    <t>SE</t>
+  </si>
+  <si>
+    <t>SI</t>
+  </si>
+  <si>
+    <t>UK</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -136,6 +156,15 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -417,14 +446,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -435,272 +466,282 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="n">
+      <c r="B2">
         <v>4</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2">
         <v>23</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="n">
+      <c r="B3">
         <v>77</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3">
         <v>89</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="n">
+      <c r="B4">
         <v>107</v>
       </c>
-      <c r="C4" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5">
+      <c r="C4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="n">
+      <c r="B5">
         <v>420</v>
       </c>
-      <c r="C5" t="n">
+      <c r="C5">
         <v>27</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" t="n">
+      <c r="B6">
         <v>311</v>
       </c>
-      <c r="C6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7">
+      <c r="C6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="B7" t="n">
+      <c r="B7">
         <v>108</v>
       </c>
-      <c r="C7" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8">
+      <c r="C7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
-      <c r="B8" t="n">
+      <c r="B8">
         <v>897</v>
       </c>
-      <c r="C8" t="n">
+      <c r="C8">
         <v>45</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
-      <c r="B9" t="n">
+      <c r="B9">
         <v>1042</v>
       </c>
-      <c r="C9" t="n">
+      <c r="C9">
         <v>463</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>11</v>
       </c>
-      <c r="B10" t="n">
+      <c r="B10">
         <v>736</v>
       </c>
-      <c r="C10" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11">
+      <c r="C10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>12</v>
       </c>
-      <c r="B11" t="n">
+      <c r="B11">
         <v>584</v>
       </c>
-      <c r="C11" t="n">
+      <c r="C11">
         <v>235</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>13</v>
       </c>
-      <c r="B12" t="n">
+      <c r="B12">
         <v>92</v>
       </c>
-      <c r="C12" t="n">
+      <c r="C12">
         <v>122</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>14</v>
       </c>
-      <c r="B13" t="n">
+      <c r="B13">
         <v>169</v>
       </c>
-      <c r="C13" t="n">
+      <c r="C13">
         <v>292</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>15</v>
       </c>
-      <c r="B14" t="n">
+      <c r="B14">
         <v>339</v>
       </c>
-      <c r="C14" t="n">
+      <c r="C14">
         <v>141</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>16</v>
       </c>
-      <c r="B15" t="n">
+      <c r="B15">
         <v>10</v>
       </c>
-      <c r="C15" t="n">
+      <c r="C15">
         <v>20</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>17</v>
       </c>
-      <c r="B16" t="n">
+      <c r="B16">
         <v>14</v>
       </c>
-      <c r="C16" t="n">
+      <c r="C16">
         <v>7</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>18</v>
       </c>
-      <c r="B17" t="n">
+      <c r="B17">
         <v>50</v>
       </c>
-      <c r="C17" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18">
+      <c r="C17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>19</v>
       </c>
-      <c r="B18" t="n">
+      <c r="B18">
         <v>47</v>
       </c>
-      <c r="C18" t="n">
+      <c r="C18">
         <v>37</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>20</v>
       </c>
-      <c r="B19" t="n">
+      <c r="B19">
         <v>459</v>
       </c>
-      <c r="C19" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20">
+      <c r="C19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>21</v>
       </c>
-      <c r="B20" t="n">
+      <c r="B20">
         <v>46</v>
       </c>
-      <c r="C20" t="n">
+      <c r="C20">
         <v>32</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>22</v>
       </c>
-      <c r="B21" t="n">
+      <c r="B21">
         <v>309</v>
       </c>
-      <c r="C21" t="n">
+      <c r="C21">
         <v>236</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>23</v>
       </c>
-      <c r="B22" t="n">
+      <c r="B22">
         <v>20</v>
       </c>
-      <c r="C22" t="n">
+      <c r="C22">
         <v>9</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>24</v>
       </c>
-      <c r="B23" t="n">
+      <c r="B23">
         <v>1539</v>
       </c>
-      <c r="C23" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24">
+      <c r="C23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>25</v>
       </c>
-      <c r="B24" t="n">
+      <c r="B24">
         <v>13</v>
       </c>
-      <c r="C24" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25">
+      <c r="C24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>26</v>
       </c>
-      <c r="B25" t="n">
+      <c r="B25">
         <v>3166</v>
       </c>
-      <c r="C25" t="n">
+      <c r="C25">
         <v>758</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B27">
+        <f>SUM(B2:B26)</f>
+        <v>10559</v>
+      </c>
+      <c r="C27">
+        <f>SUM(C2:C26)</f>
+        <v>2536</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>